<commit_message>
add swimming pool comparison for pumped hydro problem and updated ensemble forecast for wind analysis
</commit_message>
<xml_diff>
--- a/Pumped_Hydro_Example.xlsx
+++ b/Pumped_Hydro_Example.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16300" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="26660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t xml:space="preserve">How many cubic meters of reservoir storage needed to produce 1 KWh?  </t>
   </si>
@@ -70,6 +70,18 @@
   </si>
   <si>
     <t>Joule=(kg)*(m/s^2)*(m)</t>
+  </si>
+  <si>
+    <t>m^3</t>
+  </si>
+  <si>
+    <t>5 MWh storage equals:</t>
+  </si>
+  <si>
+    <t>Olympic swimming pools</t>
+  </si>
+  <si>
+    <t>volume of olympic swimming pool</t>
   </si>
 </sst>
 </file>
@@ -125,8 +137,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -136,9 +150,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -468,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -509,7 +525,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="1">
-        <v>0.72</v>
+        <v>0.9</v>
       </c>
       <c r="C4" s="1"/>
     </row>
@@ -590,10 +606,43 @@
       </c>
       <c r="B12" s="1">
         <f>B7*B8/(B4*B3*B5)</f>
-        <v>5000.0000000000009</v>
+        <v>4000</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <f>2500</f>
+        <v>2500</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <f>B12/B6*5000</f>
+        <v>20000</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <f>SUM(B15)</f>
+        <v>20000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add final wind analysis project statement from MECE 4210 Energy Infrastructure Planning
</commit_message>
<xml_diff>
--- a/Pumped_Hydro_Example.xlsx
+++ b/Pumped_Hydro_Example.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="26660" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -484,7 +484,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
@@ -495,12 +495,12 @@
     <col min="1" max="1" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -509,7 +509,7 @@
       </c>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -520,7 +520,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -529,7 +529,7 @@
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -540,7 +540,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -551,7 +551,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -560,7 +560,7 @@
       </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -570,14 +570,14 @@
       </c>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
@@ -588,7 +588,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
@@ -600,7 +600,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -612,7 +612,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -624,7 +624,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -635,14 +635,18 @@
       <c r="C15" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="D15">
+        <f>(B15)^(1/3)</f>
+        <v>27.144176165949055</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>19</v>
       </c>
       <c r="B16">
-        <f>SUM(B15)</f>
-        <v>20000</v>
+        <f>B15/B13</f>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>